<commit_message>
download format(prf and email)
</commit_message>
<xml_diff>
--- a/excel/export.xlsx
+++ b/excel/export.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="EvaluationForm" sheetId="1" r:id="rId4"/>
+    <sheet name="PRF format" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0"/>
@@ -15,63 +15,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
-  <si>
-    <t>PRF-POSITION-INSTANCE-ROUND</t>
-  </si>
-  <si>
-    <t>Full Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Functional/Technical Knowledge</t>
-  </si>
-  <si>
-    <t>Relevant Project/Functional Experience</t>
-  </si>
-  <si>
-    <t>Major Strengths(Technical/Functional)</t>
-  </si>
-  <si>
-    <t>Major Weaknesses(Technical/Functional)</t>
-  </si>
-  <si>
-    <t>Any special areas probes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Result Of Interview </t>
-  </si>
-  <si>
-    <t>If on-hold (Reason)</t>
-  </si>
-  <si>
-    <t>If selected (Designation)</t>
-  </si>
-  <si>
-    <t>If selected (Joining Date)</t>
-  </si>
-  <si>
-    <t>Remarks, if any</t>
-  </si>
-  <si>
-    <t>441194-01-001-01</t>
-  </si>
-  <si>
-    <t>Atharva  Deshpande</t>
-  </si>
-  <si>
-    <t>asdeshpande@mitaoe.ac.in</t>
-  </si>
-  <si>
-    <t>Excellent</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>selected</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+  <si>
+    <t>Instance ID</t>
+  </si>
+  <si>
+    <t>Instance Name</t>
+  </si>
+  <si>
+    <t>Submissiong Date</t>
+  </si>
+  <si>
+    <t>Requester</t>
+  </si>
+  <si>
+    <t>Position Details</t>
+  </si>
+  <si>
+    <t>Production Line</t>
+  </si>
+  <si>
+    <t>Hiring Type</t>
+  </si>
+  <si>
+    <t>Classification 100</t>
+  </si>
+  <si>
+    <t>Classification 110</t>
+  </si>
+  <si>
+    <t>Classification 111</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>Cost Center Name</t>
+  </si>
+  <si>
+    <t>Cost Center Code</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Number of Position Open</t>
+  </si>
+  <si>
+    <t>Workforce Classification</t>
+  </si>
+  <si>
+    <t>Request Type</t>
+  </si>
+  <si>
+    <t>Employee Code &amp; 8ID</t>
+  </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>New Joiner 8 ID</t>
+  </si>
+  <si>
+    <t>New Joiner Name</t>
+  </si>
+  <si>
+    <t>Required Date</t>
+  </si>
+  <si>
+    <t>Reporting To</t>
+  </si>
+  <si>
+    <t>Budget CTC in INR (Including Perks, Allownaces, benefits, etc)</t>
+  </si>
+  <si>
+    <t>Internal Posting Recommended</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Next Handler</t>
   </si>
 </sst>
 </file>
@@ -427,10 +457,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:YZ2"/>
+  <dimension ref="A1:YZ1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="BZ1" sqref="BZ1"/>
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1153,112 +1183,53 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
-      <c r="AN1" s="1"/>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1"/>
-      <c r="AQ1" s="1"/>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1"/>
-      <c r="AT1" s="1"/>
-      <c r="AU1" s="1"/>
-      <c r="AV1" s="1"/>
-      <c r="AW1" s="1"/>
-      <c r="AX1" s="1"/>
-      <c r="AY1" s="1"/>
-      <c r="AZ1" s="1"/>
-      <c r="BA1" s="1"/>
-      <c r="BB1" s="1"/>
-      <c r="BC1" s="1"/>
-      <c r="BD1" s="1"/>
-      <c r="BE1" s="1"/>
-      <c r="BF1" s="1"/>
-      <c r="BG1" s="1"/>
-      <c r="BH1" s="1"/>
-      <c r="BI1" s="1"/>
-      <c r="BJ1" s="1"/>
-      <c r="BK1" s="1"/>
-      <c r="BL1" s="1"/>
-      <c r="BM1" s="1"/>
-      <c r="BN1" s="1"/>
-      <c r="BO1" s="1"/>
-      <c r="BP1" s="1"/>
-      <c r="BQ1" s="1"/>
-      <c r="BR1" s="1"/>
-      <c r="BS1" s="1"/>
-      <c r="BT1" s="1"/>
-      <c r="BU1" s="1"/>
-      <c r="BV1" s="1"/>
-      <c r="BW1" s="1"/>
-      <c r="BX1" s="1"/>
-      <c r="BY1" s="1"/>
-      <c r="BZ1" s="1"/>
-    </row>
-    <row r="2" spans="1:676">
-      <c r="A2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2"/>
-      <c r="K2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" t="s">
-        <v>14</v>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>